<commit_message>
user dashborad response file change
</commit_message>
<xml_diff>
--- a/public/retailer/Eligible Retailer List (2022-06-15).xlsx
+++ b/public/retailer/Eligible Retailer List (2022-06-15).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Sr.</t>
   </si>
@@ -85,7 +85,7 @@
     <t>Proprietor</t>
   </si>
   <si>
-    <t>0100000000002577</t>
+    <t>0100000000002132</t>
   </si>
   <si>
     <t>1234567890123</t>
@@ -115,7 +115,7 @@
     <t>DHK-99-92</t>
   </si>
   <si>
-    <t>0100000000003569</t>
+    <t>0100000000003947</t>
   </si>
   <si>
     <t>1234567890124</t>
@@ -133,7 +133,7 @@
     <t>DHK-99-94</t>
   </si>
   <si>
-    <t>0100000000004335</t>
+    <t>0100000000004714</t>
   </si>
   <si>
     <t>1234567890125</t>
@@ -157,7 +157,7 @@
     <t>Wholesaler</t>
   </si>
   <si>
-    <t>0100000000005398</t>
+    <t>0100000000005612</t>
   </si>
   <si>
     <t>1234567890126</t>
@@ -175,13 +175,52 @@
     <t>DHK-99-98</t>
   </si>
   <si>
-    <t>0100000000006154</t>
+    <t>0100000000006989</t>
   </si>
   <si>
     <t>1234567890127</t>
   </si>
   <si>
     <t>Karim</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Coca</t>
+  </si>
+  <si>
+    <t>01711546789</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0100000000007290</t>
+  </si>
+  <si>
+    <t>1234567890760</t>
+  </si>
+  <si>
+    <t>Karim Coca</t>
+  </si>
+  <si>
+    <t>Sprite</t>
+  </si>
+  <si>
+    <t>01711098764</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0100000000008590</t>
+  </si>
+  <si>
+    <t>1234567890090</t>
+  </si>
+  <si>
+    <t>Karim  Sprite</t>
   </si>
 </sst>
 </file>
@@ -243,7 +282,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -597,9 +636,127 @@
         <v>29</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="S6" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>8765098764</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1234567897603</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>1234567671</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>4673209876</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>1234567895610</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>1234567894</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="S8" s="0" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>